<commit_message>
Adicionando docstrings no crud e aprimorando schemas
</commit_message>
<xml_diff>
--- a/documentos/editaveis/Requisitos.xlsx
+++ b/documentos/editaveis/Requisitos.xlsx
@@ -494,7 +494,7 @@
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" hidden="1">
+    <row r="2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -509,7 +509,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" hidden="1">
+    <row r="3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -524,7 +524,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" hidden="1">
+    <row r="4">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -539,7 +539,7 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" hidden="1">
+    <row r="5">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -554,7 +554,7 @@
       </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" hidden="1">
+    <row r="6">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -569,7 +569,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" hidden="1">
+    <row r="7">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -584,7 +584,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" hidden="1">
+    <row r="8">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -599,7 +599,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" hidden="1">
+    <row r="9">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -617,7 +617,7 @@
       <c r="G9" s="8"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" hidden="1">
+    <row r="10">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Atualizando documentos para suportar dois tipos de usuario
</commit_message>
<xml_diff>
--- a/documentos/editaveis/Requisitos.xlsx
+++ b/documentos/editaveis/Requisitos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">O sistema deverá permitir a listagem de produtos com os relativos códigos, nomes, quantidades e valores. Também deve permitir a filtragem de acordo com nome, código e seus classificadores (categoria, marca e máquina). </t>
+  </si>
+  <si>
+    <t>Administrador, Financeiro</t>
   </si>
   <si>
     <t>RF03</t>
@@ -173,7 +176,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -181,14 +184,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -211,47 +229,68 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FFC6C6C6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC6C6C6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -473,7 +512,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="9.63"/>
     <col customWidth="1" min="2" max="2" width="21.25"/>
-    <col customWidth="1" min="3" max="3" width="47.38"/>
+    <col customWidth="1" min="3" max="3" width="61.75"/>
     <col customWidth="1" min="4" max="5" width="25.38"/>
     <col customWidth="1" min="7" max="7" width="28.13"/>
     <col customWidth="1" min="8" max="8" width="23.63"/>
@@ -486,259 +525,267 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
+      <c r="C9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
+      <c r="C10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="B11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
+      <c r="C11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="B12" s="11" t="s">
         <v>37</v>
       </c>
+      <c r="C12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="12"/>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
+      <c r="C13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14">
-      <c r="A14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
+      <c r="C14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="B15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
+      <c r="C15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16">
-      <c r="A16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
+      <c r="C16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="10"/>
     </row>
     <row r="17">
-      <c r="A17" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
+      <c r="B17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="10"/>
     </row>
     <row r="18">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="11"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="19">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="11"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="14"/>
     </row>
   </sheetData>
   <printOptions gridLines="1" horizontalCentered="1"/>

</xml_diff>